<commit_message>
Rename from Lab 1 to Lab 2
</commit_message>
<xml_diff>
--- a/resources/complexity_summary.xlsx
+++ b/resources/complexity_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/PycharmProjects/PRasmussenLab1/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/PycharmProjects/PRasmussenLab2/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A57BA3-9311-9843-90AB-B4E04FDBBF93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A62635F-1FFE-614E-AF07-440409891699}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E21E846-EB35-BE42-9386-6F847BA31100}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27340" windowHeight="17500" xr2:uid="{4E21E846-EB35-BE42-9386-6F847BA31100}"/>
   </bookViews>
   <sheets>
     <sheet name="complexity_summary" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
-    <t>Peter Rasmussen, Lab 1</t>
-  </si>
-  <si>
     <t>convert_prefix_input</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Peter Rasmussen, Lab 2</t>
   </si>
 </sst>
 </file>
@@ -2633,7 +2633,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2648,26 +2648,26 @@
   <sheetData>
     <row r="2" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>100</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>1000</v>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>10000</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>10</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
         <v>50</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
         <v>100</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
         <v>500</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>1000</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>10000</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>10</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
         <v>50</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>100</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>500</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>1000</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
         <v>10000</v>

</xml_diff>